<commit_message>
fix algortme & all program
</commit_message>
<xml_diff>
--- a/Program Test -----/sample_data.xlsx
+++ b/Program Test -----/sample_data.xlsx
@@ -446,7 +446,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,10 +468,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -479,21 +479,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
@@ -501,32 +501,32 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>11</v>

</xml_diff>